<commit_message>
integrated iclabel and rectify channels
</commit_message>
<xml_diff>
--- a/eeg_tools/operations.xlsx
+++ b/eeg_tools/operations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\work-matlab\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\behaviourPlatform\CommonScript\eeg\eeg_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11490" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="subject" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
   <si>
     <t>do_import</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>STILL MISSING</t>
+  </si>
+  <si>
+    <t>do_iclabel</t>
+  </si>
+  <si>
+    <t>apply iclabel and icflag tools for independent components classification and possible automatic removal</t>
   </si>
 </sst>
 </file>
@@ -729,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +772,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A39" si="0">A2+1</f>
+        <f t="shared" ref="A3:A40" si="0">A2+1</f>
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1004,16 +1010,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,10 +1028,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1034,10 +1040,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +1052,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1058,10 +1064,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1070,10 +1076,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,10 +1088,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,10 +1100,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1106,10 +1112,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,10 +1124,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,10 +1136,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1142,10 +1148,10 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,10 +1160,10 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1166,10 +1172,10 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,10 +1184,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,10 +1196,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1202,9 +1208,21 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1217,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new functions to compare erp/ersp between conditions at subject level, to export data to / process with ragu; fix microstates for both continuous and epoched data; channel rectification; trigger extraction using an analog signal/channel (based on a threshold and/or deflection durartions)
</commit_message>
<xml_diff>
--- a/eeg_tools/operations.xlsx
+++ b/eeg_tools/operations.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
   <si>
     <t>do_import</t>
   </si>
@@ -415,6 +415,72 @@
   </si>
   <si>
     <t>apply iclabel and icflag tools for independent components classification and possible automatic removal</t>
+  </si>
+  <si>
+    <t>do_compute_hr</t>
+  </si>
+  <si>
+    <t>compute heart rate from EKG channel and add it as a channel</t>
+  </si>
+  <si>
+    <t>do_cleanline</t>
+  </si>
+  <si>
+    <t>cleanline</t>
+  </si>
+  <si>
+    <t>do_recover_asr</t>
+  </si>
+  <si>
+    <t>recover asr cleaned file</t>
+  </si>
+  <si>
+    <t>do_darbeliai_export2ragu</t>
+  </si>
+  <si>
+    <t>do_ragu</t>
+  </si>
+  <si>
+    <t>export data from eeglab to ragu</t>
+  </si>
+  <si>
+    <t>process data with ragu</t>
+  </si>
+  <si>
+    <t>do_export_data</t>
+  </si>
+  <si>
+    <t>export data in standard formats like EDF</t>
+  </si>
+  <si>
+    <t>do_subject_erp_curve</t>
+  </si>
+  <si>
+    <t>plot comparison of erp curve between conditions for single subject</t>
+  </si>
+  <si>
+    <t>do_subject_erp_topo</t>
+  </si>
+  <si>
+    <t>plot comparison of erp topographic map between conditions for single subject</t>
+  </si>
+  <si>
+    <t>do_subject_ersp_tf</t>
+  </si>
+  <si>
+    <t>plot comparison of ersp time-frequency representation between conditions for single subject</t>
+  </si>
+  <si>
+    <t>do_extract_trigger_duration</t>
+  </si>
+  <si>
+    <t>extract /identify triggers from one channel using deflection durations</t>
+  </si>
+  <si>
+    <t>do_extract_trigger_evaluate</t>
+  </si>
+  <si>
+    <t>extract /identify triggers from one channel (using its deflections) which are bounded between couples of events and evaluate delayes between events and extracted trigger onsets</t>
   </si>
 </sst>
 </file>
@@ -735,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A40"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,52 +836,52 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A40" si="0">A2+1</f>
+        <f t="shared" ref="A3:A51" si="0">A2+1</f>
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -824,46 +890,46 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -872,10 +938,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -884,10 +950,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -896,106 +962,106 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1004,10 +1070,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1016,34 +1082,34 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1052,22 +1118,22 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1076,10 +1142,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,10 +1154,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,10 +1166,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,10 +1178,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,10 +1190,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,22 +1202,22 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,10 +1226,10 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1172,10 +1238,10 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,10 +1250,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,10 +1262,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,10 +1274,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,10 +1286,142 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compatibility with eeglab 2021.1
</commit_message>
<xml_diff>
--- a/eeg_tools/operations.xlsx
+++ b/eeg_tools/operations.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="154">
   <si>
     <t>do_import</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>extract /identify triggers from one channel (using its deflections) which are bounded between couples of events and evaluate delayes between events and extracted trigger onsets</t>
+  </si>
+  <si>
+    <t>do_amica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amica and save backup file _icabck with ica decomposition </t>
   </si>
 </sst>
 </file>
@@ -801,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +844,7 @@
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A51" si="0">A2+1</f>
+        <f t="shared" ref="A3:A52" si="0">A2+1</f>
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1112,40 +1118,40 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,10 +1160,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1166,10 +1172,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,10 +1184,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,10 +1196,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1202,34 +1208,34 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1238,10 +1244,10 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,10 +1256,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,10 +1268,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1274,10 +1280,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,10 +1292,10 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1298,10 +1304,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,10 +1316,10 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1322,10 +1328,10 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,10 +1340,10 @@
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,10 +1352,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1358,10 +1364,10 @@
         <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1370,10 +1376,10 @@
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,22 +1388,22 @@
         <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1406,21 +1412,33 @@
         <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>